<commit_message>
Updated Manufacturing files for the purpose of having JLC attach passive components to the PCB
</commit_message>
<xml_diff>
--- a/Documents/BOM V3/Music_Visualizer_BOM_Digikey_Final_V3.xlsx
+++ b/Documents/BOM V3/Music_Visualizer_BOM_Digikey_Final_V3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ECE_Projects\Music_Visualizer\Documents\BOM V3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5005CE4D-D7ED-439D-9B6A-8C8A2628F384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E18E8F-7A70-431B-A70B-C36552FDB4A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22920" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Music_Visualizer" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="462" uniqueCount="391">
   <si>
     <t>Comment</t>
   </si>
@@ -89,9 +89,6 @@
     <t>1n</t>
   </si>
   <si>
-    <t>C21,C22,C25,C26,C27,C28,C29,C30,C31,C32,C33,C34,C35,C36,C37,C38,C39,C40,C41,C42</t>
-  </si>
-  <si>
     <t>3n</t>
   </si>
   <si>
@@ -1208,16 +1205,7 @@
     <t>KAF15AR71H273JM</t>
   </si>
   <si>
-    <t>R41 and R50 are fine</t>
-  </si>
-  <si>
-    <t>R34 is fine</t>
-  </si>
-  <si>
-    <t>C58: 1.7uF</t>
-  </si>
-  <si>
-    <t>R48 is fine</t>
+    <t>C21,C22,C25,C26,C27,C28,C29,C30,C31,C32,C33,C34,C35,C36,C37,C38,C41,C42</t>
   </si>
 </sst>
 </file>
@@ -1710,13 +1698,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2074,13 +2060,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J78"/>
+  <dimension ref="A1:I78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B53" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B83" sqref="B83"/>
+      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2095,7 +2081,7 @@
     <col min="9" max="9" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2106,25 +2092,25 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E1" t="s">
         <v>155</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>156</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>157</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>158</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>159</v>
       </c>
-      <c r="I1" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2139,10 +2125,10 @@
         <v>2</v>
       </c>
       <c r="E2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F2" t="s">
         <v>161</v>
-      </c>
-      <c r="F2" t="s">
-        <v>162</v>
       </c>
       <c r="G2" s="2">
         <v>0.1</v>
@@ -2152,10 +2138,10 @@
         <v>0.2</v>
       </c>
       <c r="I2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2170,10 +2156,10 @@
         <v>2</v>
       </c>
       <c r="E3" t="s">
+        <v>163</v>
+      </c>
+      <c r="F3" t="s">
         <v>164</v>
-      </c>
-      <c r="F3" t="s">
-        <v>165</v>
       </c>
       <c r="G3" s="2">
         <v>0.43</v>
@@ -2183,10 +2169,10 @@
         <v>0.86</v>
       </c>
       <c r="I3" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -2201,10 +2187,10 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
+        <v>172</v>
+      </c>
+      <c r="F4" t="s">
         <v>173</v>
-      </c>
-      <c r="F4" t="s">
-        <v>174</v>
       </c>
       <c r="G4" s="2">
         <v>0.1</v>
@@ -2214,10 +2200,10 @@
         <v>0.2</v>
       </c>
       <c r="I4" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -2232,10 +2218,10 @@
         <v>2</v>
       </c>
       <c r="E5" t="s">
+        <v>175</v>
+      </c>
+      <c r="F5" t="s">
         <v>176</v>
-      </c>
-      <c r="F5" t="s">
-        <v>177</v>
       </c>
       <c r="G5" s="2">
         <v>0.1</v>
@@ -2245,10 +2231,10 @@
         <v>0.2</v>
       </c>
       <c r="I5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -2263,10 +2249,10 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
+        <v>166</v>
+      </c>
+      <c r="F6" t="s">
         <v>167</v>
-      </c>
-      <c r="F6" t="s">
-        <v>168</v>
       </c>
       <c r="G6" s="2">
         <v>0.41</v>
@@ -2276,10 +2262,10 @@
         <v>0.82</v>
       </c>
       <c r="I6" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -2294,10 +2280,10 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
+        <v>169</v>
+      </c>
+      <c r="F7" t="s">
         <v>170</v>
-      </c>
-      <c r="F7" t="s">
-        <v>171</v>
       </c>
       <c r="G7" s="2">
         <v>0.18</v>
@@ -2307,46 +2293,46 @@
         <v>0.36</v>
       </c>
       <c r="I7" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>390</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E8" t="s">
+        <v>178</v>
+      </c>
+      <c r="F8" t="s">
         <v>179</v>
-      </c>
-      <c r="F8" t="s">
-        <v>180</v>
       </c>
       <c r="G8" s="2">
         <v>0.1</v>
       </c>
       <c r="H8" s="2">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="I8" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
         <v>19</v>
-      </c>
-      <c r="B9" t="s">
-        <v>20</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -2356,10 +2342,10 @@
         <v>2</v>
       </c>
       <c r="E9" t="s">
+        <v>370</v>
+      </c>
+      <c r="F9" t="s">
         <v>371</v>
-      </c>
-      <c r="F9" t="s">
-        <v>372</v>
       </c>
       <c r="G9" s="2">
         <v>0.11</v>
@@ -2369,15 +2355,15 @@
         <v>0.22</v>
       </c>
       <c r="I9" t="s">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
         <v>21</v>
-      </c>
-      <c r="B10" t="s">
-        <v>22</v>
       </c>
       <c r="C10" t="s">
         <v>5</v>
@@ -2387,10 +2373,10 @@
         <v>2</v>
       </c>
       <c r="E10" t="s">
+        <v>388</v>
+      </c>
+      <c r="F10" t="s">
         <v>389</v>
-      </c>
-      <c r="F10" t="s">
-        <v>390</v>
       </c>
       <c r="G10" s="2">
         <v>0.18</v>
@@ -2400,15 +2386,15 @@
         <v>0.36</v>
       </c>
       <c r="I10" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
+        <v>379</v>
+      </c>
+      <c r="B11" t="s">
         <v>380</v>
-      </c>
-      <c r="B11" t="s">
-        <v>381</v>
       </c>
       <c r="C11" t="s">
         <v>5</v>
@@ -2417,10 +2403,10 @@
         <v>2</v>
       </c>
       <c r="E11" t="s">
+        <v>384</v>
+      </c>
+      <c r="F11" t="s">
         <v>385</v>
-      </c>
-      <c r="F11" t="s">
-        <v>386</v>
       </c>
       <c r="G11" s="2">
         <v>0.14000000000000001</v>
@@ -2430,28 +2416,28 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="I11" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
         <v>23</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>24</v>
       </c>
-      <c r="C12" t="s">
-        <v>25</v>
-      </c>
       <c r="D12" s="1">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E12" t="s">
+        <v>350</v>
+      </c>
+      <c r="F12" t="s">
         <v>351</v>
-      </c>
-      <c r="F12" t="s">
-        <v>352</v>
       </c>
       <c r="G12" s="2">
         <v>0.56000000000000005</v>
@@ -2461,15 +2447,15 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="I12" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
         <v>26</v>
-      </c>
-      <c r="B13" t="s">
-        <v>27</v>
       </c>
       <c r="C13" t="s">
         <v>8</v>
@@ -2479,10 +2465,10 @@
         <v>3</v>
       </c>
       <c r="E13" t="s">
+        <v>353</v>
+      </c>
+      <c r="F13" t="s">
         <v>354</v>
-      </c>
-      <c r="F13" t="s">
-        <v>355</v>
       </c>
       <c r="G13" s="2">
         <v>0.14000000000000001</v>
@@ -2492,15 +2478,15 @@
         <v>0.42000000000000004</v>
       </c>
       <c r="I13" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
         <v>28</v>
-      </c>
-      <c r="B14" t="s">
-        <v>29</v>
       </c>
       <c r="C14" t="s">
         <v>5</v>
@@ -2510,10 +2496,10 @@
         <v>7</v>
       </c>
       <c r="E14" t="s">
+        <v>373</v>
+      </c>
+      <c r="F14" t="s">
         <v>374</v>
-      </c>
-      <c r="F14" t="s">
-        <v>375</v>
       </c>
       <c r="G14" s="2">
         <v>0.34</v>
@@ -2523,31 +2509,28 @@
         <v>2.3800000000000003</v>
       </c>
       <c r="I14" t="s">
-        <v>376</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
         <v>30</v>
       </c>
-      <c r="B15" t="s">
-        <v>31</v>
-      </c>
       <c r="C15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E15" t="s">
+        <v>356</v>
+      </c>
+      <c r="F15" t="s">
         <v>357</v>
-      </c>
-      <c r="F15" t="s">
-        <v>358</v>
       </c>
       <c r="G15" s="2">
         <v>0.53</v>
@@ -2557,15 +2540,15 @@
         <v>1.06</v>
       </c>
       <c r="I15" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
         <v>32</v>
-      </c>
-      <c r="B16" t="s">
-        <v>33</v>
       </c>
       <c r="C16" t="s">
         <v>5</v>
@@ -2575,7 +2558,7 @@
         <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="F16">
         <v>885012206074</v>
@@ -2588,15 +2571,15 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="I16" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
         <v>34</v>
-      </c>
-      <c r="B17" t="s">
-        <v>35</v>
       </c>
       <c r="C17" t="s">
         <v>5</v>
@@ -2606,10 +2589,10 @@
         <v>1</v>
       </c>
       <c r="E17" t="s">
+        <v>376</v>
+      </c>
+      <c r="F17" t="s">
         <v>377</v>
-      </c>
-      <c r="F17" t="s">
-        <v>378</v>
       </c>
       <c r="G17" s="2">
         <v>0.1</v>
@@ -2619,15 +2602,15 @@
         <v>0.1</v>
       </c>
       <c r="I17" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
         <v>36</v>
-      </c>
-      <c r="B18" t="s">
-        <v>37</v>
       </c>
       <c r="C18" t="s">
         <v>8</v>
@@ -2637,10 +2620,10 @@
         <v>15</v>
       </c>
       <c r="E18" t="s">
+        <v>361</v>
+      </c>
+      <c r="F18" t="s">
         <v>362</v>
-      </c>
-      <c r="F18" t="s">
-        <v>363</v>
       </c>
       <c r="G18" s="2">
         <v>0.14000000000000001</v>
@@ -2650,15 +2633,15 @@
         <v>2.1</v>
       </c>
       <c r="I18" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
         <v>38</v>
-      </c>
-      <c r="B19" t="s">
-        <v>39</v>
       </c>
       <c r="C19" t="s">
         <v>8</v>
@@ -2668,10 +2651,10 @@
         <v>2</v>
       </c>
       <c r="E19" t="s">
+        <v>364</v>
+      </c>
+      <c r="F19" t="s">
         <v>365</v>
-      </c>
-      <c r="F19" t="s">
-        <v>366</v>
       </c>
       <c r="G19" s="2">
         <v>0.36</v>
@@ -2681,15 +2664,15 @@
         <v>0.72</v>
       </c>
       <c r="I19" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" t="s">
         <v>40</v>
-      </c>
-      <c r="B20" t="s">
-        <v>41</v>
       </c>
       <c r="C20" t="s">
         <v>8</v>
@@ -2699,10 +2682,10 @@
         <v>2</v>
       </c>
       <c r="E20" t="s">
+        <v>367</v>
+      </c>
+      <c r="F20" t="s">
         <v>368</v>
-      </c>
-      <c r="F20" t="s">
-        <v>369</v>
       </c>
       <c r="G20" s="2">
         <v>0.36</v>
@@ -2712,59 +2695,59 @@
         <v>0.72</v>
       </c>
       <c r="I20" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" t="s">
         <v>42</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
+        <v>334</v>
+      </c>
+      <c r="D21" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>181</v>
+      </c>
+      <c r="F21" t="s">
+        <v>182</v>
+      </c>
+      <c r="G21" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="I21" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="A22" t="s">
         <v>43</v>
       </c>
-      <c r="C21" t="s">
-        <v>335</v>
-      </c>
-      <c r="D21" s="1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E21" t="s">
-        <v>182</v>
-      </c>
-      <c r="F21" t="s">
-        <v>183</v>
-      </c>
-      <c r="G21" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H21" s="2">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="I21" t="s">
+      <c r="B22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" t="s">
+        <v>334</v>
+      </c>
+      <c r="D22" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E22" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" t="s">
-        <v>335</v>
-      </c>
-      <c r="D22" s="1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>185</v>
-      </c>
-      <c r="F22" t="s">
-        <v>186</v>
       </c>
       <c r="G22" s="2">
         <v>0.15</v>
@@ -2774,121 +2757,121 @@
         <v>0.15</v>
       </c>
       <c r="I22" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" t="s">
+        <v>334</v>
+      </c>
+      <c r="D23" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="F23" t="s">
+        <v>188</v>
+      </c>
+      <c r="G23" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H23" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="I23" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="A24" t="s">
         <v>47</v>
       </c>
-      <c r="C23" t="s">
-        <v>335</v>
-      </c>
-      <c r="D23" s="1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E23" t="s">
-        <v>188</v>
-      </c>
-      <c r="F23" t="s">
-        <v>189</v>
-      </c>
-      <c r="G23" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H23" s="2">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="I23" t="s">
+      <c r="B24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" t="s">
+        <v>334</v>
+      </c>
+      <c r="D24" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
-        <v>48</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="F24" t="s">
+        <v>191</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H24" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="I24" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="A25" t="s">
         <v>49</v>
       </c>
-      <c r="C24" t="s">
-        <v>335</v>
-      </c>
-      <c r="D24" s="1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E24" t="s">
-        <v>191</v>
-      </c>
-      <c r="F24" t="s">
-        <v>192</v>
-      </c>
-      <c r="G24" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H24" s="2">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="I24" t="s">
+      <c r="B25" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" t="s">
+        <v>334</v>
+      </c>
+      <c r="D25" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="F25" t="s">
+        <v>194</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H25" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="I25" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="A26" t="s">
         <v>51</v>
       </c>
-      <c r="C25" t="s">
-        <v>335</v>
-      </c>
-      <c r="D25" s="1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E25" t="s">
-        <v>194</v>
-      </c>
-      <c r="F25" t="s">
-        <v>195</v>
-      </c>
-      <c r="G25" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H25" s="2">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="I25" t="s">
+      <c r="B26" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" t="s">
+        <v>334</v>
+      </c>
+      <c r="D26" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
-        <v>52</v>
-      </c>
-      <c r="B26" t="s">
-        <v>53</v>
-      </c>
-      <c r="C26" t="s">
-        <v>335</v>
-      </c>
-      <c r="D26" s="1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>197</v>
-      </c>
-      <c r="F26" t="s">
-        <v>198</v>
       </c>
       <c r="G26" s="2">
         <v>0.15</v>
@@ -2898,1060 +2881,1051 @@
         <v>0.15</v>
       </c>
       <c r="I26" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" t="s">
+        <v>334</v>
+      </c>
+      <c r="D27" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
-      <c r="A27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="F27" t="s">
+        <v>200</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H27" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="I27" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="A28" t="s">
         <v>55</v>
       </c>
-      <c r="C27" t="s">
-        <v>335</v>
-      </c>
-      <c r="D27" s="1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E27" t="s">
-        <v>200</v>
-      </c>
-      <c r="F27" t="s">
-        <v>201</v>
-      </c>
-      <c r="G27" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H27" s="2">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="I27" t="s">
+      <c r="B28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C28" t="s">
+        <v>334</v>
+      </c>
+      <c r="D28" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
-        <v>56</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="F28" t="s">
+        <v>203</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H28" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="I28" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
         <v>57</v>
       </c>
-      <c r="C28" t="s">
-        <v>335</v>
-      </c>
-      <c r="D28" s="1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E28" t="s">
-        <v>203</v>
-      </c>
-      <c r="F28" t="s">
-        <v>204</v>
-      </c>
-      <c r="G28" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H28" s="2">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="I28" t="s">
+      <c r="B29" t="s">
+        <v>58</v>
+      </c>
+      <c r="C29" t="s">
+        <v>334</v>
+      </c>
+      <c r="D29" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E29" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
-        <v>58</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="F29" t="s">
+        <v>206</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H29" s="2">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="I29" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="A30" t="s">
         <v>59</v>
       </c>
-      <c r="C29" t="s">
-        <v>335</v>
-      </c>
-      <c r="D29" s="1">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="E29" t="s">
-        <v>206</v>
-      </c>
-      <c r="F29" t="s">
-        <v>207</v>
-      </c>
-      <c r="G29" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H29" s="2">
-        <f t="shared" si="0"/>
-        <v>0.6</v>
-      </c>
-      <c r="I29" t="s">
+      <c r="B30" t="s">
+        <v>60</v>
+      </c>
+      <c r="C30" t="s">
+        <v>334</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
-        <v>60</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="F30" t="s">
+        <v>209</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H30" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="I30" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
         <v>61</v>
       </c>
-      <c r="C30" t="s">
-        <v>335</v>
-      </c>
-      <c r="D30" s="1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E30" t="s">
-        <v>209</v>
-      </c>
-      <c r="F30" t="s">
-        <v>210</v>
-      </c>
-      <c r="G30" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H30" s="2">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="I30" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
+      <c r="B31" t="s">
         <v>62</v>
       </c>
-      <c r="B31" t="s">
-        <v>63</v>
-      </c>
       <c r="C31" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D31" s="1">
         <f>LEN(B31)-LEN(SUBSTITUTE(B31,",",""))+1</f>
         <v>3</v>
       </c>
       <c r="E31" t="s">
+        <v>211</v>
+      </c>
+      <c r="F31" t="s">
         <v>212</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" si="0"/>
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="I31" t="s">
         <v>213</v>
       </c>
-      <c r="G31" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H31" s="2">
+    </row>
+    <row r="32" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" t="s">
+        <v>334</v>
+      </c>
+      <c r="D32" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>214</v>
+      </c>
+      <c r="F32" t="s">
+        <v>215</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H32" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="I32" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="A33" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" t="s">
+        <v>334</v>
+      </c>
+      <c r="D33" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>217</v>
+      </c>
+      <c r="F33" t="s">
+        <v>218</v>
+      </c>
+      <c r="G33" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H33" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="I33" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="A34" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" t="s">
+        <v>334</v>
+      </c>
+      <c r="D34" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E34" t="s">
+        <v>220</v>
+      </c>
+      <c r="F34" t="s">
+        <v>221</v>
+      </c>
+      <c r="G34" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H34" s="2">
         <f t="shared" si="0"/>
         <v>0.44999999999999996</v>
       </c>
-      <c r="I31" t="s">
-        <v>214</v>
-      </c>
-      <c r="J31" s="4" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
-        <v>64</v>
-      </c>
-      <c r="B32" t="s">
-        <v>65</v>
-      </c>
-      <c r="C32" t="s">
-        <v>335</v>
-      </c>
-      <c r="D32" s="1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E32" t="s">
-        <v>215</v>
-      </c>
-      <c r="F32" t="s">
-        <v>216</v>
-      </c>
-      <c r="G32" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H32" s="2">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="I32" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
-      <c r="A33" t="s">
-        <v>66</v>
-      </c>
-      <c r="B33" t="s">
-        <v>67</v>
-      </c>
-      <c r="C33" t="s">
-        <v>335</v>
-      </c>
-      <c r="D33" s="1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E33" t="s">
-        <v>218</v>
-      </c>
-      <c r="F33" t="s">
-        <v>219</v>
-      </c>
-      <c r="G33" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H33" s="2">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="I33" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
-      <c r="A34" t="s">
-        <v>68</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="I34" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="A35" t="s">
         <v>69</v>
       </c>
-      <c r="C34" t="s">
-        <v>335</v>
-      </c>
-      <c r="D34" s="1">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="E34" t="s">
-        <v>221</v>
-      </c>
-      <c r="F34" t="s">
-        <v>222</v>
-      </c>
-      <c r="G34" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H34" s="2">
-        <f t="shared" si="0"/>
-        <v>0.44999999999999996</v>
-      </c>
-      <c r="I34" t="s">
+      <c r="B35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" t="s">
+        <v>334</v>
+      </c>
+      <c r="D35" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="35" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
-        <v>70</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="F35" t="s">
+        <v>224</v>
+      </c>
+      <c r="G35" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H35" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="I35" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="A36" t="s">
         <v>71</v>
       </c>
-      <c r="C35" t="s">
-        <v>335</v>
-      </c>
-      <c r="D35" s="1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E35" t="s">
-        <v>224</v>
-      </c>
-      <c r="F35" t="s">
-        <v>225</v>
-      </c>
-      <c r="G35" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H35" s="2">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="I35" t="s">
+      <c r="B36" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" t="s">
+        <v>334</v>
+      </c>
+      <c r="D36" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E36" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="36" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
-      <c r="A36" t="s">
-        <v>72</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="F36" t="s">
+        <v>227</v>
+      </c>
+      <c r="G36" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H36" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="I36" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="A37" t="s">
         <v>73</v>
       </c>
-      <c r="C36" t="s">
-        <v>335</v>
-      </c>
-      <c r="D36" s="1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E36" t="s">
-        <v>227</v>
-      </c>
-      <c r="F36" t="s">
-        <v>228</v>
-      </c>
-      <c r="G36" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H36" s="2">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="I36" t="s">
+      <c r="B37" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" t="s">
+        <v>334</v>
+      </c>
+      <c r="D37" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="37" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
-      <c r="A37" t="s">
-        <v>74</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="F37" t="s">
+        <v>230</v>
+      </c>
+      <c r="G37" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H37" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="I37" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="A38" t="s">
         <v>75</v>
       </c>
-      <c r="C37" t="s">
-        <v>335</v>
-      </c>
-      <c r="D37" s="1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E37" t="s">
-        <v>230</v>
-      </c>
-      <c r="F37" t="s">
-        <v>231</v>
-      </c>
-      <c r="G37" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H37" s="2">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="I37" t="s">
+      <c r="B38" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" t="s">
+        <v>334</v>
+      </c>
+      <c r="D38" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E38" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="38" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
-      <c r="A38" t="s">
-        <v>76</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="F38" t="s">
+        <v>233</v>
+      </c>
+      <c r="G38" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H38" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="I38" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="A39" t="s">
         <v>77</v>
       </c>
-      <c r="C38" t="s">
-        <v>335</v>
-      </c>
-      <c r="D38" s="1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E38" t="s">
-        <v>233</v>
-      </c>
-      <c r="F38" t="s">
-        <v>234</v>
-      </c>
-      <c r="G38" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H38" s="2">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="I38" t="s">
+      <c r="B39" t="s">
+        <v>78</v>
+      </c>
+      <c r="C39" t="s">
+        <v>334</v>
+      </c>
+      <c r="D39" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E39" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
-      <c r="A39" t="s">
-        <v>78</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="F39" t="s">
+        <v>236</v>
+      </c>
+      <c r="G39" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H39" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="I39" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="A40" t="s">
         <v>79</v>
       </c>
-      <c r="C39" t="s">
-        <v>335</v>
-      </c>
-      <c r="D39" s="1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E39" t="s">
-        <v>236</v>
-      </c>
-      <c r="F39" t="s">
-        <v>237</v>
-      </c>
-      <c r="G39" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H39" s="2">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="I39" t="s">
+      <c r="B40" t="s">
+        <v>80</v>
+      </c>
+      <c r="C40" t="s">
+        <v>334</v>
+      </c>
+      <c r="D40" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E40" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
-      <c r="A40" t="s">
-        <v>80</v>
-      </c>
-      <c r="B40" t="s">
+      <c r="F40" t="s">
+        <v>239</v>
+      </c>
+      <c r="G40" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H40" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="I40" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="A41" t="s">
         <v>81</v>
       </c>
-      <c r="C40" t="s">
-        <v>335</v>
-      </c>
-      <c r="D40" s="1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E40" t="s">
-        <v>239</v>
-      </c>
-      <c r="F40" t="s">
-        <v>240</v>
-      </c>
-      <c r="G40" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H40" s="2">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="I40" t="s">
+      <c r="B41" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" t="s">
+        <v>334</v>
+      </c>
+      <c r="D41" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E41" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="41" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
-      <c r="A41" t="s">
-        <v>82</v>
-      </c>
-      <c r="B41" t="s">
+      <c r="F41" t="s">
+        <v>242</v>
+      </c>
+      <c r="G41" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H41" s="2">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="I41" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="A42" t="s">
         <v>83</v>
       </c>
-      <c r="C41" t="s">
-        <v>335</v>
-      </c>
-      <c r="D41" s="1">
+      <c r="B42" t="s">
+        <v>84</v>
+      </c>
+      <c r="C42" t="s">
+        <v>334</v>
+      </c>
+      <c r="D42" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E42" t="s">
+        <v>244</v>
+      </c>
+      <c r="F42" t="s">
+        <v>245</v>
+      </c>
+      <c r="G42" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H42" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="I42" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="A43" t="s">
+        <v>85</v>
+      </c>
+      <c r="B43" t="s">
+        <v>86</v>
+      </c>
+      <c r="C43" t="s">
+        <v>334</v>
+      </c>
+      <c r="D43" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E43" t="s">
+        <v>247</v>
+      </c>
+      <c r="F43" t="s">
+        <v>248</v>
+      </c>
+      <c r="G43" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H43" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="I43" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="A44" t="s">
+        <v>87</v>
+      </c>
+      <c r="B44" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" t="s">
+        <v>334</v>
+      </c>
+      <c r="D44" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E44" t="s">
+        <v>250</v>
+      </c>
+      <c r="F44" t="s">
+        <v>251</v>
+      </c>
+      <c r="G44" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H44" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="I44" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45" t="s">
+        <v>90</v>
+      </c>
+      <c r="C45" t="s">
+        <v>334</v>
+      </c>
+      <c r="D45" s="1">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="E41" t="s">
-        <v>242</v>
-      </c>
-      <c r="F41" t="s">
-        <v>243</v>
-      </c>
-      <c r="G41" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H41" s="2">
+      <c r="E45" t="s">
+        <v>253</v>
+      </c>
+      <c r="F45" t="s">
+        <v>254</v>
+      </c>
+      <c r="G45" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H45" s="2">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
-      <c r="I41" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
-      <c r="A42" t="s">
-        <v>84</v>
-      </c>
-      <c r="B42" t="s">
-        <v>85</v>
-      </c>
-      <c r="C42" t="s">
-        <v>335</v>
-      </c>
-      <c r="D42" s="1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E42" t="s">
-        <v>245</v>
-      </c>
-      <c r="F42" t="s">
-        <v>246</v>
-      </c>
-      <c r="G42" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H42" s="2">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="I42" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
-      <c r="A43" t="s">
-        <v>86</v>
-      </c>
-      <c r="B43" t="s">
-        <v>87</v>
-      </c>
-      <c r="C43" t="s">
-        <v>335</v>
-      </c>
-      <c r="D43" s="1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E43" t="s">
-        <v>248</v>
-      </c>
-      <c r="F43" t="s">
-        <v>249</v>
-      </c>
-      <c r="G43" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H43" s="2">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="I43" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
-      <c r="A44" t="s">
-        <v>88</v>
-      </c>
-      <c r="B44" t="s">
-        <v>89</v>
-      </c>
-      <c r="C44" t="s">
-        <v>335</v>
-      </c>
-      <c r="D44" s="1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E44" t="s">
-        <v>251</v>
-      </c>
-      <c r="F44" t="s">
-        <v>252</v>
-      </c>
-      <c r="G44" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H44" s="2">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="I44" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
-      <c r="A45" t="s">
-        <v>90</v>
-      </c>
-      <c r="B45" t="s">
+      <c r="I45" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="A46" t="s">
         <v>91</v>
       </c>
-      <c r="C45" t="s">
-        <v>335</v>
-      </c>
-      <c r="D45" s="1">
+      <c r="B46" t="s">
+        <v>92</v>
+      </c>
+      <c r="C46" t="s">
+        <v>334</v>
+      </c>
+      <c r="D46" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E46" t="s">
+        <v>256</v>
+      </c>
+      <c r="F46" t="s">
+        <v>257</v>
+      </c>
+      <c r="G46" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H46" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="I46" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="A47" t="s">
+        <v>93</v>
+      </c>
+      <c r="B47" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" t="s">
+        <v>334</v>
+      </c>
+      <c r="D47" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="E47" t="s">
+        <v>259</v>
+      </c>
+      <c r="F47" t="s">
+        <v>260</v>
+      </c>
+      <c r="G47" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H47" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="I47" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
+      <c r="A48" t="s">
+        <v>95</v>
+      </c>
+      <c r="B48" t="s">
+        <v>96</v>
+      </c>
+      <c r="C48" t="s">
+        <v>334</v>
+      </c>
+      <c r="D48" s="1">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="E45" t="s">
-        <v>254</v>
-      </c>
-      <c r="F45" t="s">
-        <v>255</v>
-      </c>
-      <c r="G45" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H45" s="2">
+      <c r="E48" t="s">
+        <v>262</v>
+      </c>
+      <c r="F48" t="s">
+        <v>263</v>
+      </c>
+      <c r="G48" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H48" s="2">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
-      <c r="I45" t="s">
-        <v>256</v>
-      </c>
-      <c r="J45" s="4" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
-      <c r="A46" t="s">
-        <v>92</v>
-      </c>
-      <c r="B46" t="s">
-        <v>93</v>
-      </c>
-      <c r="C46" t="s">
-        <v>335</v>
-      </c>
-      <c r="D46" s="1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E46" t="s">
-        <v>257</v>
-      </c>
-      <c r="F46" t="s">
-        <v>258</v>
-      </c>
-      <c r="G46" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H46" s="2">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="I46" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
-      <c r="A47" t="s">
-        <v>94</v>
-      </c>
-      <c r="B47" t="s">
-        <v>95</v>
-      </c>
-      <c r="C47" t="s">
-        <v>335</v>
-      </c>
-      <c r="D47" s="1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="E47" t="s">
-        <v>260</v>
-      </c>
-      <c r="F47" t="s">
-        <v>261</v>
-      </c>
-      <c r="G47" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H47" s="2">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="I47" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="16.8" x14ac:dyDescent="0.45">
-      <c r="A48" t="s">
-        <v>96</v>
-      </c>
-      <c r="B48" t="s">
-        <v>97</v>
-      </c>
-      <c r="C48" t="s">
-        <v>335</v>
-      </c>
-      <c r="D48" s="1">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="E48" t="s">
-        <v>263</v>
-      </c>
-      <c r="F48" t="s">
+      <c r="I48" t="s">
         <v>264</v>
-      </c>
-      <c r="G48" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H48" s="2">
-        <f t="shared" si="0"/>
-        <v>0.3</v>
-      </c>
-      <c r="I48" t="s">
-        <v>265</v>
-      </c>
-      <c r="J48" s="4" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
+        <v>97</v>
+      </c>
+      <c r="B49" t="s">
         <v>98</v>
       </c>
-      <c r="B49" t="s">
-        <v>99</v>
-      </c>
       <c r="C49" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D49" s="1">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="E49" t="s">
+        <v>265</v>
+      </c>
+      <c r="F49" t="s">
         <v>266</v>
       </c>
-      <c r="F49" t="s">
+      <c r="G49" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H49" s="2">
+        <f t="shared" si="0"/>
+        <v>0.44999999999999996</v>
+      </c>
+      <c r="I49" t="s">
         <v>267</v>
-      </c>
-      <c r="G49" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H49" s="2">
-        <f t="shared" si="0"/>
-        <v>0.44999999999999996</v>
-      </c>
-      <c r="I49" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
+        <v>99</v>
+      </c>
+      <c r="B50" t="s">
         <v>100</v>
       </c>
-      <c r="B50" t="s">
-        <v>101</v>
-      </c>
       <c r="C50" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D50" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E50" t="s">
+        <v>268</v>
+      </c>
+      <c r="F50" t="s">
         <v>269</v>
       </c>
-      <c r="F50" t="s">
+      <c r="G50" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H50" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="I50" t="s">
         <v>270</v>
-      </c>
-      <c r="G50" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H50" s="2">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="I50" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
+        <v>101</v>
+      </c>
+      <c r="B51" t="s">
         <v>102</v>
       </c>
-      <c r="B51" t="s">
-        <v>103</v>
-      </c>
       <c r="C51" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D51" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E51" t="s">
+        <v>271</v>
+      </c>
+      <c r="F51" t="s">
         <v>272</v>
       </c>
-      <c r="F51" t="s">
+      <c r="G51" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H51" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="I51" t="s">
         <v>273</v>
-      </c>
-      <c r="G51" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H51" s="2">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="I51" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
+        <v>103</v>
+      </c>
+      <c r="B52" t="s">
         <v>104</v>
       </c>
-      <c r="B52" t="s">
-        <v>105</v>
-      </c>
       <c r="C52" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D52" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E52" t="s">
+        <v>274</v>
+      </c>
+      <c r="F52" t="s">
         <v>275</v>
       </c>
-      <c r="F52" t="s">
+      <c r="G52" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H52" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="I52" t="s">
         <v>276</v>
-      </c>
-      <c r="G52" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H52" s="2">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="I52" t="s">
-        <v>277</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
+        <v>105</v>
+      </c>
+      <c r="B53" t="s">
         <v>106</v>
       </c>
-      <c r="B53" t="s">
-        <v>107</v>
-      </c>
       <c r="C53" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D53" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E53" t="s">
+        <v>277</v>
+      </c>
+      <c r="F53" t="s">
         <v>278</v>
       </c>
-      <c r="F53" t="s">
+      <c r="G53" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H53" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="I53" t="s">
         <v>279</v>
-      </c>
-      <c r="G53" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H53" s="2">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="I53" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
+        <v>107</v>
+      </c>
+      <c r="B54" t="s">
         <v>108</v>
       </c>
-      <c r="B54" t="s">
-        <v>109</v>
-      </c>
       <c r="C54" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D54" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E54" t="s">
+        <v>280</v>
+      </c>
+      <c r="F54" t="s">
         <v>281</v>
       </c>
-      <c r="F54" t="s">
+      <c r="G54" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H54" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="I54" t="s">
         <v>282</v>
-      </c>
-      <c r="G54" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H54" s="2">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="I54" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
+        <v>109</v>
+      </c>
+      <c r="B55" t="s">
         <v>110</v>
       </c>
-      <c r="B55" t="s">
-        <v>111</v>
-      </c>
       <c r="C55" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D55" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E55" t="s">
+        <v>283</v>
+      </c>
+      <c r="F55" t="s">
         <v>284</v>
       </c>
-      <c r="F55" t="s">
+      <c r="G55" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H55" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="I55" t="s">
         <v>285</v>
-      </c>
-      <c r="G55" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H55" s="2">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="I55" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
+        <v>111</v>
+      </c>
+      <c r="B56" t="s">
         <v>112</v>
       </c>
-      <c r="B56" t="s">
-        <v>113</v>
-      </c>
       <c r="C56" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D56" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E56" t="s">
+        <v>286</v>
+      </c>
+      <c r="F56" t="s">
         <v>287</v>
       </c>
-      <c r="F56" t="s">
+      <c r="G56" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H56" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="I56" t="s">
         <v>288</v>
-      </c>
-      <c r="G56" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H56" s="2">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="I56" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
+        <v>113</v>
+      </c>
+      <c r="B57" t="s">
         <v>114</v>
       </c>
-      <c r="B57" t="s">
-        <v>115</v>
-      </c>
       <c r="C57" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D57" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E57" t="s">
+        <v>289</v>
+      </c>
+      <c r="F57" t="s">
         <v>290</v>
       </c>
-      <c r="F57" t="s">
+      <c r="G57" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H57" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="I57" t="s">
         <v>291</v>
-      </c>
-      <c r="G57" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H57" s="2">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="I57" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
+        <v>115</v>
+      </c>
+      <c r="B58" t="s">
         <v>116</v>
       </c>
-      <c r="B58" t="s">
-        <v>117</v>
-      </c>
       <c r="C58" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D58" s="1">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="E58" t="s">
+        <v>292</v>
+      </c>
+      <c r="F58" t="s">
         <v>293</v>
       </c>
-      <c r="F58" t="s">
+      <c r="G58" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H58" s="2">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="I58" t="s">
         <v>294</v>
-      </c>
-      <c r="G58" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H58" s="2">
-        <f t="shared" si="0"/>
-        <v>0.3</v>
-      </c>
-      <c r="I58" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
+        <v>117</v>
+      </c>
+      <c r="B59" t="s">
         <v>118</v>
       </c>
-      <c r="B59" t="s">
-        <v>119</v>
-      </c>
       <c r="C59" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D59" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="E59" t="s">
+        <v>295</v>
+      </c>
+      <c r="F59" t="s">
         <v>296</v>
       </c>
-      <c r="F59" t="s">
+      <c r="G59" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="H59" s="2">
+        <f t="shared" si="0"/>
+        <v>0.15</v>
+      </c>
+      <c r="I59" t="s">
         <v>297</v>
-      </c>
-      <c r="G59" s="2">
-        <v>0.15</v>
-      </c>
-      <c r="H59" s="2">
-        <f t="shared" si="0"/>
-        <v>0.15</v>
-      </c>
-      <c r="I59" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
+        <v>119</v>
+      </c>
+      <c r="B60" t="s">
         <v>120</v>
       </c>
-      <c r="B60" t="s">
-        <v>121</v>
-      </c>
       <c r="C60" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D60" s="1">
         <f t="shared" ref="D60:D62" si="2">LEN(B60)-LEN(SUBSTITUTE(B60,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="E60" t="s">
+        <v>298</v>
+      </c>
+      <c r="F60" t="s">
         <v>299</v>
-      </c>
-      <c r="F60" t="s">
-        <v>300</v>
       </c>
       <c r="G60" s="2">
         <v>0.15</v>
@@ -3961,28 +3935,28 @@
         <v>0.15</v>
       </c>
       <c r="I60" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
+        <v>121</v>
+      </c>
+      <c r="B61" t="s">
         <v>122</v>
       </c>
-      <c r="B61" t="s">
-        <v>123</v>
-      </c>
       <c r="C61" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D61" s="1">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E61" t="s">
+        <v>301</v>
+      </c>
+      <c r="F61" t="s">
         <v>302</v>
-      </c>
-      <c r="F61" t="s">
-        <v>303</v>
       </c>
       <c r="G61" s="2">
         <v>0.15</v>
@@ -3992,28 +3966,28 @@
         <v>0.15</v>
       </c>
       <c r="I61" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
+        <v>123</v>
+      </c>
+      <c r="B62" t="s">
         <v>124</v>
       </c>
-      <c r="B62" t="s">
-        <v>125</v>
-      </c>
       <c r="C62" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D62" s="1">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="E62" t="s">
+        <v>304</v>
+      </c>
+      <c r="F62" t="s">
         <v>305</v>
-      </c>
-      <c r="F62" t="s">
-        <v>306</v>
       </c>
       <c r="G62" s="2">
         <v>0.15</v>
@@ -4023,28 +3997,28 @@
         <v>0.15</v>
       </c>
       <c r="I62" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
+        <v>125</v>
+      </c>
+      <c r="B63" t="s">
         <v>126</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C63" t="s">
         <v>127</v>
-      </c>
-      <c r="C63" t="s">
-        <v>128</v>
       </c>
       <c r="D63" s="1">
         <f>LEN(B63)-LEN(SUBSTITUTE(B63,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="E63" t="s">
+        <v>307</v>
+      </c>
+      <c r="F63" t="s">
         <v>308</v>
-      </c>
-      <c r="F63" t="s">
-        <v>309</v>
       </c>
       <c r="G63" s="2">
         <v>0.15</v>
@@ -4054,28 +4028,28 @@
         <v>0.15</v>
       </c>
       <c r="I63" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
+        <v>128</v>
+      </c>
+      <c r="B64" t="s">
         <v>129</v>
       </c>
-      <c r="B64" t="s">
-        <v>130</v>
-      </c>
       <c r="C64" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D64" s="1">
         <f t="shared" ref="D64:D77" si="4">LEN(B64)-LEN(SUBSTITUTE(B64,",",""))+1</f>
         <v>1</v>
       </c>
       <c r="E64" t="s">
+        <v>310</v>
+      </c>
+      <c r="F64" t="s">
         <v>311</v>
-      </c>
-      <c r="F64" t="s">
-        <v>312</v>
       </c>
       <c r="G64" s="2">
         <v>0.15</v>
@@ -4085,28 +4059,28 @@
         <v>0.15</v>
       </c>
       <c r="I64" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
+        <v>130</v>
+      </c>
+      <c r="B65" t="s">
         <v>131</v>
       </c>
-      <c r="B65" t="s">
-        <v>132</v>
-      </c>
       <c r="C65" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D65" s="1">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E65" t="s">
+        <v>313</v>
+      </c>
+      <c r="F65" t="s">
         <v>314</v>
-      </c>
-      <c r="F65" t="s">
-        <v>315</v>
       </c>
       <c r="G65" s="2">
         <v>0.15</v>
@@ -4116,28 +4090,28 @@
         <v>0.15</v>
       </c>
       <c r="I65" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
+        <v>132</v>
+      </c>
+      <c r="B66" t="s">
         <v>133</v>
       </c>
-      <c r="B66" t="s">
-        <v>134</v>
-      </c>
       <c r="C66" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D66" s="1">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E66" t="s">
+        <v>316</v>
+      </c>
+      <c r="F66" t="s">
         <v>317</v>
-      </c>
-      <c r="F66" t="s">
-        <v>318</v>
       </c>
       <c r="G66" s="2">
         <v>0.15</v>
@@ -4147,28 +4121,28 @@
         <v>0.15</v>
       </c>
       <c r="I66" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
+        <v>134</v>
+      </c>
+      <c r="B67" t="s">
         <v>135</v>
       </c>
-      <c r="B67" t="s">
-        <v>136</v>
-      </c>
       <c r="C67" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D67" s="1">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E67" t="s">
+        <v>319</v>
+      </c>
+      <c r="F67" t="s">
         <v>320</v>
-      </c>
-      <c r="F67" t="s">
-        <v>321</v>
       </c>
       <c r="G67" s="2">
         <v>0.15</v>
@@ -4178,28 +4152,28 @@
         <v>0.15</v>
       </c>
       <c r="I67" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
+        <v>136</v>
+      </c>
+      <c r="B68" t="s">
         <v>137</v>
       </c>
-      <c r="B68" t="s">
-        <v>138</v>
-      </c>
       <c r="C68" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D68" s="1">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E68" t="s">
+        <v>322</v>
+      </c>
+      <c r="F68" t="s">
         <v>323</v>
-      </c>
-      <c r="F68" t="s">
-        <v>324</v>
       </c>
       <c r="G68" s="2">
         <v>0.15</v>
@@ -4209,28 +4183,28 @@
         <v>0.15</v>
       </c>
       <c r="I68" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="69" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
+        <v>138</v>
+      </c>
+      <c r="B69" t="s">
         <v>139</v>
       </c>
-      <c r="B69" t="s">
-        <v>140</v>
-      </c>
       <c r="C69" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D69" s="1">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E69" t="s">
+        <v>325</v>
+      </c>
+      <c r="F69" t="s">
         <v>326</v>
-      </c>
-      <c r="F69" t="s">
-        <v>327</v>
       </c>
       <c r="G69" s="2">
         <v>0.15</v>
@@ -4240,28 +4214,28 @@
         <v>0.15</v>
       </c>
       <c r="I69" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
+        <v>140</v>
+      </c>
+      <c r="B70" t="s">
         <v>141</v>
       </c>
-      <c r="B70" t="s">
-        <v>142</v>
-      </c>
       <c r="C70" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D70" s="1">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="E70" t="s">
+        <v>328</v>
+      </c>
+      <c r="F70" t="s">
         <v>329</v>
-      </c>
-      <c r="F70" t="s">
-        <v>330</v>
       </c>
       <c r="G70" s="2">
         <v>0.15</v>
@@ -4271,28 +4245,28 @@
         <v>1.05</v>
       </c>
       <c r="I70" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
+        <v>142</v>
+      </c>
+      <c r="B71" t="s">
         <v>143</v>
       </c>
-      <c r="B71" t="s">
-        <v>144</v>
-      </c>
       <c r="C71" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D71" s="1">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E71" t="s">
+        <v>331</v>
+      </c>
+      <c r="F71" t="s">
         <v>332</v>
-      </c>
-      <c r="F71" t="s">
-        <v>333</v>
       </c>
       <c r="G71" s="2">
         <v>0.15</v>
@@ -4302,28 +4276,28 @@
         <v>0.15</v>
       </c>
       <c r="I71" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
+        <v>144</v>
+      </c>
+      <c r="B72" t="s">
         <v>145</v>
       </c>
-      <c r="B72" t="s">
-        <v>146</v>
-      </c>
       <c r="C72" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D72" s="1">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E72" t="s">
+        <v>335</v>
+      </c>
+      <c r="F72" t="s">
         <v>336</v>
-      </c>
-      <c r="F72" t="s">
-        <v>337</v>
       </c>
       <c r="G72" s="2">
         <v>0.15</v>
@@ -4333,28 +4307,28 @@
         <v>0.15</v>
       </c>
       <c r="I72" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="73" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
+        <v>146</v>
+      </c>
+      <c r="B73" t="s">
         <v>147</v>
       </c>
-      <c r="B73" t="s">
-        <v>148</v>
-      </c>
       <c r="C73" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D73" s="1">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E73" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F73" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G73" s="2">
         <v>0.15</v>
@@ -4364,7 +4338,7 @@
         <v>0.15</v>
       </c>
       <c r="I73" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="74" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
@@ -4372,20 +4346,20 @@
         <v>680</v>
       </c>
       <c r="B74" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C74" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D74" s="1">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="E74" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F74" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G74" s="2">
         <v>0.15</v>
@@ -4395,28 +4369,28 @@
         <v>1.05</v>
       </c>
       <c r="I74" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
+        <v>149</v>
+      </c>
+      <c r="B75" t="s">
         <v>150</v>
       </c>
-      <c r="B75" t="s">
-        <v>151</v>
-      </c>
       <c r="C75" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D75" s="1">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E75" t="s">
+        <v>344</v>
+      </c>
+      <c r="F75" t="s">
         <v>345</v>
-      </c>
-      <c r="F75" t="s">
-        <v>346</v>
       </c>
       <c r="G75" s="2">
         <v>0.15</v>
@@ -4426,7 +4400,7 @@
         <v>0.15</v>
       </c>
       <c r="I75" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
@@ -4434,20 +4408,20 @@
         <v>620</v>
       </c>
       <c r="B76" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C76" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D76">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E76" t="s">
+        <v>381</v>
+      </c>
+      <c r="F76" t="s">
         <v>382</v>
-      </c>
-      <c r="F76" t="s">
-        <v>383</v>
       </c>
       <c r="G76" s="3">
         <v>0.19</v>
@@ -4457,28 +4431,28 @@
         <v>0.19</v>
       </c>
       <c r="I76" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="77" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
+        <v>152</v>
+      </c>
+      <c r="B77" t="s">
         <v>153</v>
       </c>
-      <c r="B77" t="s">
-        <v>154</v>
-      </c>
       <c r="C77" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D77" s="1">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="E77" t="s">
+        <v>347</v>
+      </c>
+      <c r="F77" t="s">
         <v>348</v>
-      </c>
-      <c r="F77" t="s">
-        <v>349</v>
       </c>
       <c r="G77" s="2">
         <v>0.15</v>
@@ -4488,7 +4462,7 @@
         <v>0.15</v>
       </c>
       <c r="I77" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="16.8" x14ac:dyDescent="0.45">
@@ -4496,7 +4470,7 @@
       <c r="G78" s="2"/>
       <c r="H78" s="2">
         <f>SUM(H2:H77)</f>
-        <v>26.599999999999955</v>
+        <v>26.399999999999956</v>
       </c>
     </row>
   </sheetData>

</xml_diff>